<commit_message>
Add watchdog timer to main firmware FSM
</commit_message>
<xml_diff>
--- a/Sensor Node/pcb layout/sdia_profile.xlsx
+++ b/Sensor Node/pcb layout/sdia_profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshar\Documents\capstone\Sensor Node\pcb layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB4604E-F53C-4030-8A9A-617B6CB36660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DEACE4-0315-4637-95CF-5D2B6BBC8B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="10" xr2:uid="{F5149266-07BC-4AB4-837F-925A2119B882}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="8" xr2:uid="{F5149266-07BC-4AB4-837F-925A2119B882}"/>
   </bookViews>
   <sheets>
     <sheet name="sdia_profile" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Step</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Sensor Voltage</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -17580,6 +17586,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Temperature</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. RTD Voltage</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17613,7 +17649,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -17628,19 +17664,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -17722,7 +17746,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-0740-4A30-962D-FFB32CD8F907}"/>
@@ -17761,6 +17785,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>RTD Voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -17823,6 +17902,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Water Temperature</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (C)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -24582,7 +24721,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F3D62CEE-7948-48BA-9681-B24C4D9B309C}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24593,7 +24732,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D5C6AD80-CDEA-448A-8763-687477AABD52}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24813,7 +24952,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10820843" cy="7852587"/>
+    <xdr:ext cx="8661400" cy="6290733"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -24848,14 +24987,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>338137</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>261937</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:rowOff>176213</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -24887,7 +25026,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10820843" cy="7852587"/>
+    <xdr:ext cx="8661400" cy="6290733"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -39474,10 +39613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54CA122-840A-4C25-B1F1-7BE53CCE0524}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39509,6 +39648,15 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2.1123509999999999</v>
+      </c>
+      <c r="B7">
+        <f>7.2492*A7-11.198</f>
+        <v>4.1148548691999984</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39516,10 +39664,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AB6590-7759-4757-AFA2-0027578BE4A1}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39711,6 +39859,23 @@
         <v>0.12665299999999999</v>
       </c>
     </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.11951100000000001</v>
+      </c>
+      <c r="B13">
+        <f>2515.7*A13-264.78</f>
+        <v>35.873822700000005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -39721,8 +39886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8A2A2F-9BA0-4F8A-B7A2-77B4E4830BDC}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>